<commit_message>
New spreadsheet for cancel order
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupTA659.xlsx
+++ b/src/test/resources/data/jdgroupTA659.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AAA9DBB-9857-446F-8338-954BBC524749}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7044B17-E569-4BB4-A6E9-65122393667C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="24" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EVS" sheetId="82" r:id="rId1"/>
@@ -9738,8 +9738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R78" sqref="P78:R78"/>
+    <sheetView tabSelected="1" topLeftCell="N54" workbookViewId="0">
+      <selection activeCell="Q78" sqref="Q78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -15742,7 +15742,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -15865,9 +15865,10 @@
     <hyperlink ref="D4" r:id="rId9" xr:uid="{00000000-0004-0000-1100-000008000000}"/>
     <hyperlink ref="C4" r:id="rId10" xr:uid="{00000000-0004-0000-1100-000009000000}"/>
     <hyperlink ref="B2" r:id="rId11" xr:uid="{89146DFA-5225-45FC-90D8-DE1C48F64813}"/>
+    <hyperlink ref="B6" r:id="rId12" xr:uid="{06CA2C55-72F8-4103-97BD-417061DF25B3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -18391,9 +18392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58:D60"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
@@ -19503,11 +19502,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:AA102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E78" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F100" sqref="F100"/>
+      <selection pane="bottomRight" activeCell="P102" sqref="P102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -27526,9 +27525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
@@ -29101,7 +29098,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
@@ -45563,6 +45560,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -45571,7 +45577,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -45720,16 +45726,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -45737,7 +45751,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -45754,21 +45768,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>